<commit_message>
[modify] ERDiagrum and API仕様書 for Upd003
</commit_message>
<xml_diff>
--- a/20.開発/50.画面/10.画面一覧/画面一覧.xlsx
+++ b/20.開発/50.画面/10.画面一覧/画面一覧.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eternal\documents\20.開発\50.画面\10.画面一覧\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB76153-AA9A-4E2E-8DF0-181E3514B874}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1044700C-51A4-49CA-BB94-DDD840DCE360}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="変更履歴" sheetId="3" r:id="rId1"/>
@@ -20,10 +20,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">画面一覧!$B$3:$I$3</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="118">
   <si>
     <t>画面一覧</t>
     <rPh sb="0" eb="4">
@@ -347,16 +352,6 @@
   </si>
   <si>
     <t>ランキング</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Twitterの投稿蘭のイメージ</t>
-    <rPh sb="8" eb="10">
-      <t>トウコウ</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>ラン</t>
-    </rPh>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -999,6 +994,13 @@
     <t>トークテーマ投稿
 (モーダル)</t>
     <rPh sb="6" eb="8">
+      <t>トウコウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Twitterの投稿欄のイメージ</t>
+    <rPh sb="8" eb="10">
       <t>トウコウ</t>
     </rPh>
     <phoneticPr fontId="3"/>
@@ -1372,6 +1374,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1382,7 +1385,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1400,9 +1403,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
@@ -2078,32 +2080,32 @@
     <row r="1" spans="2:5" ht="8.1" customHeight="1"/>
     <row r="2" spans="2:5" ht="22.5">
       <c r="B2" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="28" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="38" t="s">
+      <c r="C3" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="D3" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="E3" s="28" t="s">
         <v>65</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="D4" s="18" t="s">
         <v>68</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>69</v>
       </c>
       <c r="E4" s="19">
         <v>43367</v>
@@ -2111,13 +2113,13 @@
     </row>
     <row r="5" spans="2:5" ht="58.5">
       <c r="B5" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E5" s="19">
         <v>43373</v>
@@ -2125,13 +2127,13 @@
     </row>
     <row r="6" spans="2:5" ht="39">
       <c r="B6" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>98</v>
-      </c>
       <c r="D6" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E6" s="19">
         <v>43380</v>
@@ -2139,13 +2141,13 @@
     </row>
     <row r="7" spans="2:5" ht="78">
       <c r="B7" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>115</v>
-      </c>
       <c r="D7" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" s="19">
         <v>43381</v>
@@ -2200,13 +2202,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>6</v>
@@ -2215,7 +2217,7 @@
         <v>8</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I3" s="12" t="s">
         <v>4</v>
@@ -2227,19 +2229,19 @@
         <v>1</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7" t="s">
@@ -2258,7 +2260,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -2272,14 +2274,14 @@
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="75">
@@ -2294,11 +2296,11 @@
         <v>11</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7" t="s">
-        <v>39</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="2:9">
@@ -2313,7 +2315,7 @@
         <v>10</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
@@ -2324,13 +2326,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>12</v>
@@ -2397,19 +2399,19 @@
         <v>10</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F13" s="25" t="s">
         <v>23</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
@@ -2443,7 +2445,7 @@
         <v>22</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -2469,19 +2471,19 @@
         <v>14</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="E17" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="E17" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="25" t="s">
-        <v>110</v>
-      </c>
       <c r="G17" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
@@ -2495,10 +2497,10 @@
       <c r="D18" s="14"/>
       <c r="E18" s="27"/>
       <c r="F18" s="25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
@@ -2509,13 +2511,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>30</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>31</v>
@@ -2539,7 +2541,7 @@
         <v>30</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
@@ -2556,7 +2558,7 @@
         <v>32</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
@@ -2570,10 +2572,10 @@
       <c r="D22" s="14"/>
       <c r="E22" s="9"/>
       <c r="F22" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>54</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
@@ -2601,23 +2603,23 @@
         <v>21</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>36</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H24" s="7"/>
-      <c r="I24" s="28" t="s">
-        <v>99</v>
+      <c r="I24" s="29" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="2:9">
@@ -2629,13 +2631,13 @@
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H25" s="7"/>
-      <c r="I25" s="29"/>
+      <c r="I25" s="30"/>
     </row>
     <row r="26" spans="2:9">
       <c r="B26" s="6">
@@ -2646,13 +2648,13 @@
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G26" s="7" t="s">
-        <v>61</v>
-      </c>
       <c r="H26" s="7"/>
-      <c r="I26" s="30"/>
+      <c r="I26" s="31"/>
     </row>
     <row r="27" spans="2:9" ht="37.5">
       <c r="B27" s="6">
@@ -2660,19 +2662,19 @@
         <v>24</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D27" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="F27" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="F27" s="6" t="s">
-        <v>85</v>
-      </c>
       <c r="G27" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
@@ -2686,10 +2688,10 @@
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="F28" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
@@ -2700,13 +2702,13 @@
         <v>26</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>25</v>
@@ -2758,16 +2760,16 @@
         <v>29</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D32" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="F32" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="G32" s="7" t="str">
         <f>G29</f>
@@ -2785,14 +2787,14 @@
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
       <c r="F33" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G33" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="75">
@@ -2801,13 +2803,13 @@
         <v>31</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>23</v>
@@ -2829,10 +2831,10 @@
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
       <c r="F35" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
@@ -2846,10 +2848,10 @@
       <c r="D36" s="23"/>
       <c r="E36" s="23"/>
       <c r="F36" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G36" s="20" t="s">
         <v>72</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>73</v>
       </c>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
@@ -2881,132 +2883,132 @@
       </c>
     </row>
     <row r="5" spans="2:32">
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="33"/>
-      <c r="O5" s="31" t="s">
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="34"/>
+      <c r="O5" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="32"/>
-      <c r="S5" s="32"/>
-      <c r="T5" s="32"/>
-      <c r="U5" s="33"/>
-      <c r="Z5" s="31" t="s">
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33"/>
+      <c r="U5" s="34"/>
+      <c r="Z5" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="AA5" s="32"/>
-      <c r="AB5" s="32"/>
-      <c r="AC5" s="32"/>
-      <c r="AD5" s="32"/>
-      <c r="AE5" s="32"/>
-      <c r="AF5" s="33"/>
+      <c r="AA5" s="33"/>
+      <c r="AB5" s="33"/>
+      <c r="AC5" s="33"/>
+      <c r="AD5" s="33"/>
+      <c r="AE5" s="33"/>
+      <c r="AF5" s="34"/>
     </row>
     <row r="6" spans="2:32">
-      <c r="D6" s="34"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="36"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="35"/>
-      <c r="S6" s="35"/>
-      <c r="T6" s="35"/>
-      <c r="U6" s="36"/>
-      <c r="Z6" s="34"/>
-      <c r="AA6" s="35"/>
-      <c r="AB6" s="35"/>
-      <c r="AC6" s="35"/>
-      <c r="AD6" s="35"/>
-      <c r="AE6" s="35"/>
-      <c r="AF6" s="36"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="37"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="36"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="36"/>
+      <c r="U6" s="37"/>
+      <c r="Z6" s="35"/>
+      <c r="AA6" s="36"/>
+      <c r="AB6" s="36"/>
+      <c r="AC6" s="36"/>
+      <c r="AD6" s="36"/>
+      <c r="AE6" s="36"/>
+      <c r="AF6" s="37"/>
     </row>
     <row r="9" spans="2:32">
-      <c r="O9" s="31" t="s">
+      <c r="O9" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="32"/>
-      <c r="S9" s="32"/>
-      <c r="T9" s="32"/>
-      <c r="U9" s="33"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="33"/>
+      <c r="S9" s="33"/>
+      <c r="T9" s="33"/>
+      <c r="U9" s="34"/>
     </row>
     <row r="10" spans="2:32">
-      <c r="O10" s="34"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="35"/>
-      <c r="R10" s="35"/>
-      <c r="S10" s="35"/>
-      <c r="T10" s="35"/>
-      <c r="U10" s="36"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="36"/>
+      <c r="Q10" s="36"/>
+      <c r="R10" s="36"/>
+      <c r="S10" s="36"/>
+      <c r="T10" s="36"/>
+      <c r="U10" s="37"/>
     </row>
     <row r="13" spans="2:32">
-      <c r="O13" s="31" t="s">
+      <c r="O13" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32"/>
-      <c r="T13" s="32"/>
-      <c r="U13" s="33"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="33"/>
+      <c r="R13" s="33"/>
+      <c r="S13" s="33"/>
+      <c r="T13" s="33"/>
+      <c r="U13" s="34"/>
     </row>
     <row r="14" spans="2:32">
-      <c r="O14" s="34"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
-      <c r="T14" s="35"/>
-      <c r="U14" s="36"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="36"/>
+      <c r="S14" s="36"/>
+      <c r="T14" s="36"/>
+      <c r="U14" s="37"/>
     </row>
     <row r="17" spans="15:32">
-      <c r="O17" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="32"/>
-      <c r="S17" s="32"/>
-      <c r="T17" s="32"/>
-      <c r="U17" s="33"/>
-      <c r="Z17" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA17" s="32"/>
-      <c r="AB17" s="32"/>
-      <c r="AC17" s="32"/>
-      <c r="AD17" s="32"/>
-      <c r="AE17" s="32"/>
-      <c r="AF17" s="33"/>
+      <c r="O17" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="33"/>
+      <c r="S17" s="33"/>
+      <c r="T17" s="33"/>
+      <c r="U17" s="34"/>
+      <c r="Z17" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA17" s="33"/>
+      <c r="AB17" s="33"/>
+      <c r="AC17" s="33"/>
+      <c r="AD17" s="33"/>
+      <c r="AE17" s="33"/>
+      <c r="AF17" s="34"/>
     </row>
     <row r="18" spans="15:32">
-      <c r="O18" s="34"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="35"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="36"/>
-      <c r="Z18" s="34"/>
-      <c r="AA18" s="35"/>
-      <c r="AB18" s="35"/>
-      <c r="AC18" s="35"/>
-      <c r="AD18" s="35"/>
-      <c r="AE18" s="35"/>
-      <c r="AF18" s="36"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="36"/>
+      <c r="U18" s="37"/>
+      <c r="Z18" s="35"/>
+      <c r="AA18" s="36"/>
+      <c r="AB18" s="36"/>
+      <c r="AC18" s="36"/>
+      <c r="AD18" s="36"/>
+      <c r="AE18" s="36"/>
+      <c r="AF18" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>